<commit_message>
edited logger readmes and added pictures
</commit_message>
<xml_diff>
--- a/01_Logger/01_Basic_Logger/02_Mechanics/BOM.xlsx
+++ b/01_Logger/01_Basic_Logger/02_Mechanics/BOM.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEC7A2D-8E80-4D96-83D5-077AC1AC4ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A313C3-B55B-4E55-B31B-8A63FB17D04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -31,12 +31,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>GTIN</t>
-  </si>
-  <si>
     <t>Mounting for electronic components, 3D printed</t>
   </si>
   <si>
@@ -49,9 +43,6 @@
     <t>Internal mounting</t>
   </si>
   <si>
-    <t>Penetrators Charging side</t>
-  </si>
-  <si>
     <t>Sensors and accessories</t>
   </si>
   <si>
@@ -67,15 +58,6 @@
     <t>Cylinder, POM, D 76/90, L 275, according to drawing</t>
   </si>
   <si>
-    <t>End cap for charing, according to drawing</t>
-  </si>
-  <si>
-    <t>Thread rod M2.5, length 75 mm</t>
-  </si>
-  <si>
-    <t>Nuts M2.5</t>
-  </si>
-  <si>
     <t>Tapping screw, M2.9 x 9.5, for attaching main PCB</t>
   </si>
   <si>
@@ -91,9 +73,6 @@
     <t>O-ring, 15.5 x 2, NBR70</t>
   </si>
   <si>
-    <t>O-ring 8.5x 1.5, NBR70</t>
-  </si>
-  <si>
     <t>Temperature: BlueRobotics Celsius Fast Responde, incl. O-ring and nut</t>
   </si>
   <si>
@@ -112,22 +91,10 @@
     <t>Pressure valve, BlueRobotics PRV-R1, incl. O-rings and nut</t>
   </si>
   <si>
-    <t>Penetrator for charging, according to drawing</t>
-  </si>
-  <si>
-    <t>Penetrator for LED, according to drawing</t>
-  </si>
-  <si>
-    <t>Nut M10, hexagonal, flat, stainless A4, DIN439/ISO4035</t>
-  </si>
-  <si>
-    <t>Washer with single head solder terminal, M2.2xM10.2, tinned copper</t>
-  </si>
-  <si>
-    <t>Mounting for reed switch incl. 1 M3x8 hex screws</t>
-  </si>
-  <si>
     <t>Bushing for conductivity sensor, incl. distance sleeve for potting</t>
+  </si>
+  <si>
+    <t>End cap, blank</t>
   </si>
 </sst>
 </file>
@@ -200,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -213,15 +180,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -504,21 +462,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E30" sqref="D30:E30"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="4.42578125" customWidth="1"/>
+    <col min="1" max="2" width="4.3984375" customWidth="1"/>
     <col min="3" max="3" width="69" style="5" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,23 +484,15 @@
       <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -552,10 +500,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -563,10 +511,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -574,10 +522,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -585,10 +533,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -596,10 +544,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -607,15 +555,15 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C9" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>7</v>
       </c>
@@ -623,10 +571,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>8</v>
       </c>
@@ -634,21 +582,21 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>10</v>
       </c>
@@ -656,37 +604,37 @@
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C14" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15">
         <v>11</v>
       </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
       <c r="B15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>13</v>
       </c>
@@ -694,10 +642,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>14</v>
       </c>
@@ -705,10 +653,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>15</v>
       </c>
@@ -716,10 +664,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>16</v>
       </c>
@@ -727,21 +675,21 @@
         <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>17</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>18</v>
       </c>
@@ -749,111 +697,18 @@
         <v>1</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>19</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>20</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>21</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>22</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>23</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>24</v>
-      </c>
-      <c r="B29">
-        <v>6</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>25</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>26</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>27</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>